<commit_message>
add param to fileData
</commit_message>
<xml_diff>
--- a/metaData.xlsx
+++ b/metaData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14310" yWindow="4455" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="14310" yWindow="4455" windowWidth="21600" windowHeight="11385" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UART message" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="129">
   <si>
     <t>ch1</t>
   </si>
@@ -361,6 +361,57 @@
   </si>
   <si>
     <t>adc3Vers</t>
+  </si>
+  <si>
+    <t>Param structure</t>
+  </si>
+  <si>
+    <t>XX</t>
+  </si>
+  <si>
+    <t>dataCH1_1</t>
+  </si>
+  <si>
+    <t>dataCH1_2</t>
+  </si>
+  <si>
+    <t>dataCH1_3</t>
+  </si>
+  <si>
+    <t>dataCH1_4</t>
+  </si>
+  <si>
+    <t>dataCH1_5</t>
+  </si>
+  <si>
+    <t>dataCH1_6</t>
+  </si>
+  <si>
+    <t>dataCH1_7</t>
+  </si>
+  <si>
+    <t>dataCH1_8</t>
+  </si>
+  <si>
+    <t>dataCH1_9</t>
+  </si>
+  <si>
+    <t>dataCH1_10</t>
+  </si>
+  <si>
+    <t>dataCH1_11</t>
+  </si>
+  <si>
+    <t>dataCH1_12</t>
+  </si>
+  <si>
+    <t>dataCH1_13</t>
+  </si>
+  <si>
+    <t>numAdcCH</t>
+  </si>
+  <si>
+    <t>1-&gt;2</t>
   </si>
 </sst>
 </file>
@@ -522,7 +573,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -587,16 +638,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -893,7 +950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AA61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Z32" sqref="Z32"/>
     </sheetView>
   </sheetViews>
@@ -912,31 +969,31 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
-      <c r="R2" s="22" t="s">
+      <c r="R2" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="S2" s="22"/>
-      <c r="T2" s="22"/>
-      <c r="U2" s="22"/>
-      <c r="V2" s="22"/>
-      <c r="W2" s="22"/>
-      <c r="X2" s="22"/>
-      <c r="Y2" s="22"/>
-      <c r="Z2" s="22"/>
-      <c r="AA2" s="22"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
@@ -962,12 +1019,12 @@
       <c r="C4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="24" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="25"/>
       <c r="F4" s="25"/>
-      <c r="G4" s="24"/>
+      <c r="G4" s="26"/>
       <c r="H4" s="13" t="s">
         <v>79</v>
       </c>
@@ -1267,16 +1324,16 @@
       <c r="F16" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="24" t="s">
         <v>18</v>
       </c>
       <c r="H16" s="25"/>
       <c r="I16" s="25"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="23" t="s">
+      <c r="J16" s="26"/>
+      <c r="K16" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="L16" s="24"/>
+      <c r="L16" s="26"/>
       <c r="M16" s="18"/>
       <c r="R16" s="13" t="s">
         <v>5</v>
@@ -1287,10 +1344,10 @@
       <c r="T16" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="U16" s="23" t="s">
+      <c r="U16" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="V16" s="24"/>
+      <c r="V16" s="26"/>
       <c r="W16" s="16"/>
       <c r="X16" s="16"/>
       <c r="Y16" s="16"/>
@@ -1378,16 +1435,16 @@
       <c r="F20" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G20" s="23" t="s">
+      <c r="G20" s="24" t="s">
         <v>18</v>
       </c>
       <c r="H20" s="25"/>
       <c r="I20" s="25"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="23" t="s">
+      <c r="J20" s="26"/>
+      <c r="K20" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="L20" s="24"/>
+      <c r="L20" s="26"/>
       <c r="R20" s="13" t="s">
         <v>5</v>
       </c>
@@ -1397,10 +1454,10 @@
       <c r="T20" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="U20" s="23" t="s">
+      <c r="U20" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="V20" s="24"/>
+      <c r="V20" s="26"/>
       <c r="W20" s="16"/>
       <c r="X20" s="16"/>
       <c r="Y20" s="16"/>
@@ -1483,16 +1540,16 @@
       <c r="F24" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G24" s="23" t="s">
+      <c r="G24" s="24" t="s">
         <v>18</v>
       </c>
       <c r="H24" s="25"/>
       <c r="I24" s="25"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="23" t="s">
+      <c r="J24" s="26"/>
+      <c r="K24" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="L24" s="24"/>
+      <c r="L24" s="26"/>
       <c r="R24" s="13" t="s">
         <v>5</v>
       </c>
@@ -1502,10 +1559,10 @@
       <c r="T24" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="U24" s="23" t="s">
+      <c r="U24" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="V24" s="24"/>
+      <c r="V24" s="26"/>
       <c r="W24" s="16"/>
       <c r="X24" s="16"/>
       <c r="Y24" s="16"/>
@@ -1587,16 +1644,16 @@
       <c r="F28" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="G28" s="23" t="s">
+      <c r="G28" s="24" t="s">
         <v>18</v>
       </c>
       <c r="H28" s="25"/>
       <c r="I28" s="25"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="23" t="s">
+      <c r="J28" s="26"/>
+      <c r="K28" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="L28" s="24"/>
+      <c r="L28" s="26"/>
       <c r="R28" s="13" t="s">
         <v>5</v>
       </c>
@@ -1606,18 +1663,18 @@
       <c r="T28" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="U28" s="23" t="s">
+      <c r="U28" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="V28" s="24"/>
-      <c r="W28" s="23" t="s">
+      <c r="V28" s="26"/>
+      <c r="W28" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="X28" s="24"/>
-      <c r="Y28" s="23" t="s">
+      <c r="X28" s="26"/>
+      <c r="Y28" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="Z28" s="24"/>
+      <c r="Z28" s="26"/>
       <c r="AA28" s="16"/>
     </row>
     <row r="29" spans="2:27" x14ac:dyDescent="0.25">
@@ -1778,12 +1835,12 @@
       <c r="U36" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="V36" s="23" t="s">
+      <c r="V36" s="24" t="s">
         <v>78</v>
       </c>
       <c r="W36" s="25"/>
       <c r="X36" s="25"/>
-      <c r="Y36" s="24"/>
+      <c r="Y36" s="26"/>
       <c r="Z36" s="15"/>
       <c r="AA36" s="15"/>
     </row>
@@ -1864,10 +1921,10 @@
       <c r="S40" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="T40" s="23" t="s">
+      <c r="T40" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="U40" s="24"/>
+      <c r="U40" s="26"/>
       <c r="V40" s="15"/>
       <c r="W40" s="15"/>
       <c r="X40" s="15"/>
@@ -1934,12 +1991,12 @@
       <c r="S44" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="T44" s="23" t="s">
+      <c r="T44" s="24" t="s">
         <v>80</v>
       </c>
       <c r="U44" s="25"/>
       <c r="V44" s="25"/>
-      <c r="W44" s="24"/>
+      <c r="W44" s="26"/>
       <c r="X44" s="13" t="s">
         <v>79</v>
       </c>
@@ -2278,12 +2335,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D4:G4"/>
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="K20:L20"/>
+    <mergeCell ref="R2:AA2"/>
+    <mergeCell ref="Y28:Z28"/>
+    <mergeCell ref="W28:X28"/>
+    <mergeCell ref="U24:V24"/>
+    <mergeCell ref="U20:V20"/>
+    <mergeCell ref="U16:V16"/>
     <mergeCell ref="T44:W44"/>
     <mergeCell ref="V36:Y36"/>
     <mergeCell ref="T40:U40"/>
@@ -2292,12 +2349,12 @@
     <mergeCell ref="G28:J28"/>
     <mergeCell ref="K28:L28"/>
     <mergeCell ref="U28:V28"/>
-    <mergeCell ref="R2:AA2"/>
-    <mergeCell ref="Y28:Z28"/>
-    <mergeCell ref="W28:X28"/>
-    <mergeCell ref="U24:V24"/>
-    <mergeCell ref="U20:V20"/>
-    <mergeCell ref="U16:V16"/>
+    <mergeCell ref="D4:G4"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="K20:L20"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2307,10 +2364,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:V11"/>
+  <dimension ref="B2:V17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2319,44 +2376,44 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
+      <c r="B2" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
     </row>
     <row r="3" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
       <c r="F3" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="H3" s="26"/>
+      <c r="H3" s="28"/>
       <c r="I3" s="4" t="s">
         <v>99</v>
       </c>
@@ -2474,11 +2531,11 @@
       <c r="V5" s="2"/>
     </row>
     <row r="6" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
       <c r="H6" s="1"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -2496,10 +2553,10 @@
       <c r="V6" s="2"/>
     </row>
     <row r="7" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="29"/>
+      <c r="C7" s="31"/>
       <c r="D7" s="3"/>
       <c r="H7" s="2"/>
       <c r="Q7" s="2"/>
@@ -2509,7 +2566,7 @@
       <c r="U7" s="2"/>
     </row>
     <row r="8" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="30" t="s">
         <v>94</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -2520,7 +2577,7 @@
       </c>
     </row>
     <row r="9" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="28"/>
+      <c r="B9" s="30"/>
       <c r="C9" s="3" t="s">
         <v>0</v>
       </c>
@@ -2537,7 +2594,7 @@
       <c r="P9" s="2"/>
     </row>
     <row r="10" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="30" t="s">
         <v>95</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -2548,7 +2605,7 @@
       </c>
     </row>
     <row r="11" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="28"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="3" t="s">
         <v>0</v>
       </c>
@@ -2556,8 +2613,199 @@
         <v>50</v>
       </c>
     </row>
+    <row r="14" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="29"/>
+    </row>
+    <row r="15" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>114</v>
+      </c>
+      <c r="G15" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="H15" s="22" t="s">
+        <v>116</v>
+      </c>
+      <c r="I15" s="22" t="s">
+        <v>117</v>
+      </c>
+      <c r="J15" s="22" t="s">
+        <v>118</v>
+      </c>
+      <c r="K15" s="22" t="s">
+        <v>119</v>
+      </c>
+      <c r="L15" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="M15" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="N15" s="22" t="s">
+        <v>122</v>
+      </c>
+      <c r="O15" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="P15" s="22" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q15" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="R15" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="S15" s="22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="L16" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="M16" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="N16" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="O16" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="P16" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="R16" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="S16" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="23">
+        <v>0</v>
+      </c>
+      <c r="C17" s="23">
+        <v>1</v>
+      </c>
+      <c r="D17" s="23">
+        <v>2</v>
+      </c>
+      <c r="E17" s="23">
+        <v>3</v>
+      </c>
+      <c r="F17" s="23">
+        <v>4</v>
+      </c>
+      <c r="G17" s="23">
+        <v>5</v>
+      </c>
+      <c r="H17" s="23">
+        <v>6</v>
+      </c>
+      <c r="I17" s="23">
+        <v>7</v>
+      </c>
+      <c r="J17" s="23">
+        <v>8</v>
+      </c>
+      <c r="K17" s="23">
+        <v>9</v>
+      </c>
+      <c r="L17" s="23">
+        <v>10</v>
+      </c>
+      <c r="M17" s="23">
+        <v>11</v>
+      </c>
+      <c r="N17" s="23">
+        <v>12</v>
+      </c>
+      <c r="O17" s="23">
+        <v>13</v>
+      </c>
+      <c r="P17" s="23">
+        <v>14</v>
+      </c>
+      <c r="Q17" s="23">
+        <v>15</v>
+      </c>
+      <c r="R17" s="23">
+        <v>16</v>
+      </c>
+      <c r="S17" s="23" t="s">
+        <v>113</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="B14:S14"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="B2:S2"/>
     <mergeCell ref="B8:B9"/>

</xml_diff>